<commit_message>
add error highlight in gender
</commit_message>
<xml_diff>
--- a/public/TestData.xlsx
+++ b/public/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jialin\Documents\GitHub\quest\frontend\src\routes\students\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jialin\Documents\GitHub\quest\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60708AB-E42E-4D04-B69D-3179E01CB745}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44407E4-2A2B-4C52-A93C-B00B1908979E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8B374D6A-B95B-45EE-AB9E-B7DA1D552B95}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Tom</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>jerry@u.nus.edu</t>
+  </si>
+  <si>
+    <t>invalid gender</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>wannasleep@u.nus.edu</t>
   </si>
 </sst>
 </file>
@@ -430,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9EF0B2-5EC9-47FD-B438-F43473A088C9}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -505,10 +514,31 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>36589</v>
+      </c>
+      <c r="D4">
+        <v>91234567</v>
+      </c>
+      <c r="E4">
+        <v>81234567</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{31EC52F9-C57A-4EAA-BF95-A134C9A837F3}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{1F257833-3EB3-490C-A109-9CECCF5FBB45}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{773A479C-477A-4708-8784-19CA6FF3B9DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>